<commit_message>
created api symlex login brand,model module pos,neg test cases
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_windows/test_cases(app)/report_summary.xlsx
+++ b/exec/symlex_vpn_windows/test_cases(app)/report_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_windows\test_cases(app)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CE00DF-4819-4E08-8AA4-002336C2F1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B527618-89CB-4D8B-A727-93B60BA4A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
@@ -22,19 +22,20 @@
     <sheet name="free_bonus" sheetId="5" r:id="rId7"/>
     <sheet name="purchase_page" sheetId="8" r:id="rId8"/>
     <sheet name="redeem_voucher" sheetId="7" r:id="rId9"/>
-    <sheet name="get_support" sheetId="16" r:id="rId10"/>
-    <sheet name="gaming_server" sheetId="15" r:id="rId11"/>
-    <sheet name="connected_devices" sheetId="14" r:id="rId12"/>
-    <sheet name="logout" sheetId="6" r:id="rId13"/>
-    <sheet name="auto_connect" sheetId="4" r:id="rId14"/>
-    <sheet name="general(settings)" sheetId="3" r:id="rId15"/>
+    <sheet name="server_list" sheetId="17" r:id="rId10"/>
+    <sheet name="get_support" sheetId="16" r:id="rId11"/>
+    <sheet name="gaming_server" sheetId="15" r:id="rId12"/>
+    <sheet name="connected_devices" sheetId="14" r:id="rId13"/>
+    <sheet name="logout" sheetId="6" r:id="rId14"/>
+    <sheet name="auto_connect" sheetId="4" r:id="rId15"/>
+    <sheet name="general(settings)" sheetId="3" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
   <si>
     <t>Features of enter vpn</t>
   </si>
@@ -177,6 +178,16 @@
   </si>
   <si>
     <t xml:space="preserve"> Test Case Summary (06-03-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_GSF_0021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (07-03-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_SP_017,
+TC_SYM_SP_029</t>
   </si>
 </sst>
 </file>
@@ -770,11 +781,80 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5D8A1E-94B5-4CB0-ACD7-301A5C4B0886}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="73.5" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F27D506-7724-410F-8C5D-BD6699CD03C2}">
   <dimension ref="D2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -795,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="4:5" ht="18.75">
@@ -811,7 +891,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="4:5" ht="18.75">
@@ -826,7 +906,9 @@
       <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -836,7 +918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345C486D-D03D-4F49-ACA7-68C5FE3BD58E}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -903,7 +985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B3D4B-C81A-4118-8051-58CD51E77CE6}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -970,7 +1052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A287E34E-8299-4D47-B00D-598C59273152}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1037,7 +1119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1106,7 +1188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G8"/>
   <sheetViews>

</xml_diff>

<commit_message>
api test case created for login osverion,osplatform,osname
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_windows/test_cases(app)/report_summary.xlsx
+++ b/exec/symlex_vpn_windows/test_cases(app)/report_summary.xlsx
@@ -8,34 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_windows\test_cases(app)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B527618-89CB-4D8B-A727-93B60BA4A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F7DB5D-CB68-4DA2-8A63-431C98C2028B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
     <sheet name="my_account" sheetId="10" r:id="rId2"/>
-    <sheet name="protocols(setting)" sheetId="9" r:id="rId3"/>
-    <sheet name="connection_page" sheetId="13" r:id="rId4"/>
-    <sheet name="ad_block_server" sheetId="12" r:id="rId5"/>
-    <sheet name="forget_password" sheetId="11" r:id="rId6"/>
-    <sheet name="free_bonus" sheetId="5" r:id="rId7"/>
-    <sheet name="purchase_page" sheetId="8" r:id="rId8"/>
-    <sheet name="redeem_voucher" sheetId="7" r:id="rId9"/>
-    <sheet name="server_list" sheetId="17" r:id="rId10"/>
-    <sheet name="get_support" sheetId="16" r:id="rId11"/>
-    <sheet name="gaming_server" sheetId="15" r:id="rId12"/>
-    <sheet name="connected_devices" sheetId="14" r:id="rId13"/>
-    <sheet name="logout" sheetId="6" r:id="rId14"/>
-    <sheet name="auto_connect" sheetId="4" r:id="rId15"/>
-    <sheet name="general(settings)" sheetId="3" r:id="rId16"/>
+    <sheet name="streaming_server" sheetId="19" r:id="rId3"/>
+    <sheet name="protocols(setting)" sheetId="9" r:id="rId4"/>
+    <sheet name="connection_page" sheetId="13" r:id="rId5"/>
+    <sheet name="ad_block_server" sheetId="12" r:id="rId6"/>
+    <sheet name="forget_password" sheetId="11" r:id="rId7"/>
+    <sheet name="free_bonus" sheetId="5" r:id="rId8"/>
+    <sheet name="purchase_page" sheetId="8" r:id="rId9"/>
+    <sheet name="redeem_voucher" sheetId="7" r:id="rId10"/>
+    <sheet name="server_list" sheetId="17" r:id="rId11"/>
+    <sheet name="get_support" sheetId="16" r:id="rId12"/>
+    <sheet name="gaming_server" sheetId="15" r:id="rId13"/>
+    <sheet name="connected_devices" sheetId="14" r:id="rId14"/>
+    <sheet name="logout" sheetId="6" r:id="rId15"/>
+    <sheet name="auto_connect" sheetId="4" r:id="rId16"/>
+    <sheet name="general(settings)" sheetId="3" r:id="rId17"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
   <si>
     <t>Features of enter vpn</t>
   </si>
@@ -188,6 +189,9 @@
   <si>
     <t>TC_SYM_SP_017,
 TC_SYM_SP_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (10-03-24)</t>
   </si>
 </sst>
 </file>
@@ -781,10 +785,79 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D112B8-BA61-4323-A81E-60AEE54129B4}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="73.5" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5D8A1E-94B5-4CB0-ACD7-301A5C4B0886}">
   <dimension ref="D2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -849,7 +922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F27D506-7724-410F-8C5D-BD6699CD03C2}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -918,7 +991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345C486D-D03D-4F49-ACA7-68C5FE3BD58E}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -985,7 +1058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B3D4B-C81A-4118-8051-58CD51E77CE6}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1052,7 +1125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A287E34E-8299-4D47-B00D-598C59273152}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1119,7 +1192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1188,7 +1261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G8"/>
   <sheetViews>
@@ -1328,6 +1401,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D08387-ADF6-4721-A906-029B94AC4100}">
+  <dimension ref="D2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:5" ht="18.75">
+      <c r="D2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="4:5" ht="18.75">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="18.75">
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18.75">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18.75">
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="73.5" customHeight="1">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9FAD35-8DBC-4806-9676-42FE393D7535}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1396,7 +1536,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0240F835-33DB-4C28-A260-ECF0731AC899}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1465,7 +1605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A33E54C-DEB5-4BB8-BB86-A2471A6B4B70}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1532,7 +1672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0FE5E3-5A70-40FA-B724-E1A08306649D}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1601,7 +1741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1670,7 +1810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20E9BD1-861C-4DAA-A578-3640159897E0}">
   <dimension ref="D2:E8"/>
   <sheetViews>
@@ -1737,73 +1877,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D112B8-BA61-4323-A81E-60AEE54129B4}">
-  <dimension ref="D2:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
-      <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="4:5" ht="18.75">
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5" ht="18.75">
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" ht="18.75">
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" ht="18.75">
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="4:5" ht="73.5" customHeight="1">
-      <c r="D8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>